<commit_message>
Final todo application code
</commit_message>
<xml_diff>
--- a/server/data/users/subbareddy.xlsx
+++ b/server/data/users/subbareddy.xlsx
@@ -398,9 +398,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -417,18 +417,32 @@
         <v>created_at</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>subbareddy</v>
+      </c>
+      <c r="B2" t="str">
+        <v>$2a$10$xIlSWnVXpCLkzt0f1HYv2.K0yPcVwAMLBQCK.2xoNlfCIk5cHRHSy</v>
+      </c>
+      <c r="C2" t="str">
+        <v>subbareddyroyal@gmail.com</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2026-01-30T14:36:29.610Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -442,18 +456,44 @@
         <v>description</v>
       </c>
       <c r="D1" t="str">
-        <v>completed</v>
+        <v>target_date</v>
       </c>
       <c r="E1" t="str">
         <v>created_at</v>
       </c>
       <c r="F1" t="str">
         <v>updated_at</v>
+      </c>
+      <c r="G1" t="str">
+        <v>completed</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>1769785959313</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Artificial intelligence</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Artificial intelligence</v>
+      </c>
+      <c r="D2" t="str">
+        <v>2026-02-28</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2026-01-30T15:12:39.313Z</v>
+      </c>
+      <c r="F2" t="str">
+        <v>2026-01-30T15:12:59.592Z</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>